<commit_message>
agent_optimized  working fine on single sheet
</commit_message>
<xml_diff>
--- a/cleaned_data.xlsx
+++ b/cleaned_data.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="$400K Media Plan" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Media Plan" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,8 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,6 +27,10 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -47,8 +52,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -123,6 +131,40 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MediaPlanTable" displayName="MediaPlanTable" ref="A1:Y8" headerRowCount="1">
+  <autoFilter ref="A1:Y8"/>
+  <tableColumns count="25">
+    <tableColumn id="1" name="Site Name"/>
+    <tableColumn id="2" name="Package Name"/>
+    <tableColumn id="3" name="Placement Name"/>
+    <tableColumn id="4" name="Audience Demo (P2+, A18-49, AA, HM)"/>
+    <tableColumn id="5" name="Audience Targeting _x000a_(ex: E! Network viewers, etc.)"/>
+    <tableColumn id="6" name="Device Type_x000a_(Mobile Web, Mobile App,  Tablet, Desktop)"/>
+    <tableColumn id="7" name="Ad Unit/Size"/>
+    <tableColumn id="8" name="Site Served Only_x000a_(Y/N)"/>
+    <tableColumn id="9" name="Buy Model"/>
+    <tableColumn id="10" name="Media Type_x000a_(Flash, Rich Media, Video Etc.)"/>
+    <tableColumn id="11" name="Start Date"/>
+    <tableColumn id="12" name="End Date"/>
+    <tableColumn id="13" name="Can be purchased on Viewability? (MOAT GroupM Viewability Standard)"/>
+    <tableColumn id="14" name="Can Utilize MOAT on this placement?_x000a_(Y/N)"/>
+    <tableColumn id="15" name="Can Purchase Programmatically? (via DV 360)  (Y/N)"/>
+    <tableColumn id="16" name="Can utilize DV on this placement?_x000a_(Y/N)"/>
+    <tableColumn id="17" name="AutoPlay or Click to Play?"/>
+    <tableColumn id="18" name="Is the Unit Skippable, Nonskippable or blended?"/>
+    <tableColumn id="19" name="Creative Restrictions (# of Swaps OR # of creative versions) per Line Item (specify # and caveat if it includes tune-in messaging)"/>
+    <tableColumn id="20" name="Rate"/>
+    <tableColumn id="21" name="Impressions"/>
+    <tableColumn id="22" name="Net Cost"/>
+    <tableColumn id="23" name="Cancellaton Date by Package"/>
+    <tableColumn id="24" name="% SOV"/>
+    <tableColumn id="25" name="Minimum package/placement amount"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,32 +456,939 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Site Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Package Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Placement Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Audience Demo (P2+, A18-49, AA, HM)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Audience Targeting 
+(ex: E! Network viewers, etc.)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Device Type
+(Mobile Web, Mobile App,  Tablet, Desktop)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Ad Unit/Size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Site Served Only
+(Y/N)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Buy Model</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Media Type
+(Flash, Rich Media, Video Etc.)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>End Date</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Can be purchased on Viewability? (MOAT GroupM Viewability Standard)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Can Utilize MOAT on this placement?
+(Y/N)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Can Purchase Programmatically? (via DV 360)  (Y/N)</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Can utilize DV on this placement?
+(Y/N)</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>AutoPlay or Click to Play?</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Is the Unit Skippable, Nonskippable or blended?</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Creative Restrictions (# of Swaps OR # of creative versions) per Line Item (specify # and caveat if it includes tune-in messaging)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Impressions</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Net Cost</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Cancellaton Date by Package</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>% SOV</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Minimum package/placement amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Samsung Ads</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CTV</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CTV Video_Lead-In_2016+ Models: 
+Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Target 1
+Viewers/Fans of The Voice (especially S26 and S27) + LALs:
+The Voice, American Idol, The Masked Singer, America's Got Talent, The X Factor, Songland, Clash of the Cover Bands, I Can See Your Voice, Name that Tune, Beat Shazam, That's My Jam
+OR
+Target 2
+Viewers/Fans of Competition Reality Shows:
+AGT (NBC &amp; Peacock), ANW (NBC &amp; Peacock), Yes Chef (NBC &amp; Peacock), American Idol (ABC), Masked Singer (FOX), The Floor (FOX) 
+OR
+Target 3
+Plus, Celebrity Talk &amp; Heartland Titles:
+Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Smart TV</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>:15/:30</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3P Tracking</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Y - Tracking Only</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>AutoPlay</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Nonskippable</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>No restrictions on # of creatives if using VAST tags</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="inlineStr">
+        <is>
+          <t>33.5</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
+          <t>5223880.6</t>
+        </is>
+      </c>
+      <c r="V2" s="3" t="inlineStr">
+        <is>
+          <t>175000.0</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>14 days</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>$10K Line Item Minimum, $75K Plan Minimum</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>First Screen Rotational</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>First Screen Rotational_Lead In_Click to Video_2017+ Models: 
+Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Target 1
+Viewers/Fans of The Voice (especially S26 and S27) + LALs:
+The Voice, American Idol, The Masked Singer, America's Got Talent, The X Factor, Songland, Clash of the Cover Bands, I Can See Your Voice, Name that Tune, Beat Shazam, That's My Jam
+OR
+Target 2
+Viewers/Fans of Competition Reality Shows:
+AGT (NBC &amp; Peacock), ANW (NBC &amp; Peacock), Yes Chef (NBC &amp; Peacock), American Idol (ABC), Masked Singer (FOX), The Floor (FOX) 
+OR
+Target 3
+Plus, Celebrity Talk &amp; Heartland Titles:
+Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smart TV </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2017+: 480x270, 960x270 + autoplay video OR 480x270, 1840x320
+Immersive: 3840 x 2160, 1824,412, 1120 x 400 (Logo)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Yes (but can be tracked by a DCM 1x1)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Custom Display</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>14.25</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>4210526.32</t>
+        </is>
+      </c>
+      <c r="V3" s="3" t="inlineStr">
+        <is>
+          <t>60000.0</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>14 days</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>$10K Line Item Minimum, $75K Plan Minimum</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>First Screen Immersive Rotational</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>'22 First Screen Immersive_Click to Video_2022-2024 Models:
+Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Target 1
+Viewers/Fans of The Voice (especially S26 and S27) + LALs:
+The Voice, American Idol, The Masked Singer, America's Got Talent, The X Factor, Songland, Clash of the Cover Bands, I Can See Your Voice, Name that Tune, Beat Shazam, That's My Jam
+OR
+Target 2
+Viewers/Fans of Competition Reality Shows:
+AGT (NBC &amp; Peacock), ANW (NBC &amp; Peacock), Yes Chef (NBC &amp; Peacock), American Idol (ABC), Masked Singer (FOX), The Floor (FOX) 
+OR
+Target 3
+Plus, Celebrity Talk &amp; Heartland Titles:
+Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smart TV </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Banner: 3840x2160
+Transparent Logo: 1120x400</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Yes (but can be tracked by a DCM 1x1)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Custom Display</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
+        </is>
+      </c>
+      <c r="T4" s="2" t="inlineStr">
+        <is>
+          <t>21.5</t>
+        </is>
+      </c>
+      <c r="U4" s="2" t="inlineStr">
+        <is>
+          <t>1860465.12</t>
+        </is>
+      </c>
+      <c r="V4" s="3" t="inlineStr">
+        <is>
+          <t>40000.0</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Non-cancellable, but can be shifted with a 60 days notice before launch </t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>$10K Line Item Minimum, $75K Plan Minimum</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>First Screen Rotational</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>First Screen Rotational_Click to App_2017+ Models: 
+Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Target 1
+Viewers/Fans of The Voice (especially S26 and S27) + LALs:
+The Voice, American Idol, The Masked Singer, America's Got Talent, The X Factor, Songland, Clash of the Cover Bands, I Can See Your Voice, Name that Tune, Beat Shazam, That's My Jam
+OR
+Target 2
+Viewers/Fans of Competition Reality Shows:
+AGT (NBC &amp; Peacock), ANW (NBC &amp; Peacock), Yes Chef (NBC &amp; Peacock), American Idol (ABC), Masked Singer (FOX), The Floor (FOX) 
+OR
+Target 3
+Plus, Celebrity Talk &amp; Heartland Titles:
+Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smart TV </t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2017+: 480x270, 960x270 + autoplay video OR 480x270, 1840x320
+Immersive: 3840 x 2160, 1824,412, 1120 x 400 (Logo)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Yes (but can be tracked by a DCM 1x1)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Custom Display</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
+        </is>
+      </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>14.25</t>
+        </is>
+      </c>
+      <c r="U5" s="2" t="inlineStr">
+        <is>
+          <t>5263157.89</t>
+        </is>
+      </c>
+      <c r="V5" s="3" t="inlineStr">
+        <is>
+          <t>75000.0</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>14 days</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>$10K Line Item Minimum, $75K Plan Minimum</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>First Screen Immersive Rotational</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>'22 First Screen Immersive_Click to App_2022-2024 Models:
+Targeting Viewers/Fans of The Voice (especially S26 and S27) + LALs, Viewers/Fans of Competition Reality Shows, Plus, Celebrity Talk &amp; Heartland Titles</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Target 1
+Viewers/Fans of The Voice (especially S26 and S27) + LALs:
+The Voice, American Idol, The Masked Singer, America's Got Talent, The X Factor, Songland, Clash of the Cover Bands, I Can See Your Voice, Name that Tune, Beat Shazam, That's My Jam
+OR
+Target 2
+Viewers/Fans of Competition Reality Shows:
+AGT (NBC &amp; Peacock), ANW (NBC &amp; Peacock), Yes Chef (NBC &amp; Peacock), American Idol (ABC), Masked Singer (FOX), The Floor (FOX) 
+OR
+Target 3
+Plus, Celebrity Talk &amp; Heartland Titles:
+Today Show (NBC &amp; Peacock), Kelly Clarkson (NBC &amp; Peacock), Yellowstone (Peacock), Days of Our Lives (Peacock)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smart TV </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Banner: 3840x2160
+Transparent Logo: 1120x400</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Yes (but can be tracked by a DCM 1x1)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Custom Display</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
+        </is>
+      </c>
+      <c r="T6" s="2" t="inlineStr">
+        <is>
+          <t>21.5</t>
+        </is>
+      </c>
+      <c r="U6" s="2" t="inlineStr">
+        <is>
+          <t>2325581.4</t>
+        </is>
+      </c>
+      <c r="V6" s="3" t="inlineStr">
+        <is>
+          <t>50000.0</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Non-cancellable, but can be shifted with a 60 days notice before launch </t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>$10K Line Item Minimum, $75K Plan Minimum</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>7.5% ADDED VALUE + 10% Buy More Get More First Screen Rotational</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Added Value (17.5%)_Native 1st Screen Ad Rotational_Lead in/Continuity_Click to Video/App: 
+Untargeted 
+9/18-9/22: Click to Video (2017+)
+9/23-10/7: Click to App (2017+)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Untargeted</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smart TV </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2017+: 480x270, 960x270 + autoplay video OR 480x270, 1840x320
+Immersive: 3840 x 2160, 1824,412, 1120 x 400 (Logo)</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Yes (but can be tracked by a DCM 1x1)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Added Value</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Custom Display</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creative restrictions are based on final budgets and flight lengths per placement </t>
+        </is>
+      </c>
+      <c r="T7" s="2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="U7" s="2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="V7" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>14 days</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="T8" s="2" t="n"/>
+      <c r="U8" s="2" t="inlineStr">
+        <is>
+          <t>18883611.33</t>
+        </is>
+      </c>
+      <c r="V8" s="3" t="inlineStr">
+        <is>
+          <t>400000.0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>